<commit_message>
Denv 1 alignment tree updated to match phylogeny from new reference set
</commit_message>
<xml_diff>
--- a/tabular/master-references-taxdata.xlsx
+++ b/tabular/master-references-taxdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/arbovirus/Dengue-GLUE-Lineages/tabular/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/arbovirus/Dengue/Dengue-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE422C7C-FBEF-0B49-9419-7AB66402CF81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68D7008-3904-DD41-86C1-7299DD956174}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10220" yWindow="500" windowWidth="17960" windowHeight="15760" xr2:uid="{D4A8156A-14E7-F041-BA15-1B362DD6A95A}"/>
   </bookViews>
@@ -80,10 +80,10 @@
     <t>3III_A</t>
   </si>
   <si>
-    <t xml:space="preserve">1IV </t>
-  </si>
-  <si>
     <t>4II</t>
+  </si>
+  <si>
+    <t>1IV</t>
   </si>
 </sst>
 </file>
@@ -469,7 +469,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="A1:F5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -546,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>1</v>
@@ -566,7 +566,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>0</v>

</xml_diff>